<commit_message>
fix: orden de las columnas de excel para copy-paste posterior
</commit_message>
<xml_diff>
--- a/output_combinado/errores_combinados.xlsx
+++ b/output_combinado/errores_combinados.xlsx
@@ -19,12 +19,12 @@
     <t>id_texto</t>
   </si>
   <si>
+    <t>errores_ortografia_literal</t>
+  </si>
+  <si>
     <t>errores_acentuales</t>
   </si>
   <si>
-    <t>errores_ortografia_literal</t>
-  </si>
-  <si>
     <t>errores_ortografia_puntual</t>
   </si>
   <si>
@@ -44,6 +44,93 @@
   </si>
   <si>
     <t>errores_cohesion_referencia</t>
+  </si>
+  <si>
+    <t>error_1: impusado → impulsado</t>
+  </si>
+  <si>
+    <t>error_1: sobretodo → sobre todo
+error_2: solidaridad  → solidaridad
+error_3: tiránica  → tiránica
+error_4: forma de vida de la personas → forma de vida de las personas</t>
+  </si>
+  <si>
+    <t>error_1: relevacia → relevancia
+error_2: debiese → debiese
+error_3: entre ello → entre ellos</t>
+  </si>
+  <si>
+    <t>error_1: llego → llegó
+error_2: frente → enfrenta
+error_3: ultimo → último
+error_4: llamo → llamó
+error_5: super → súper
+error_6: sufienciente → suficiente
+error_7: aun → aún
+error_8: tambien → también
+error_9: prodran → podrán
+error_10: asintomaticamente → asintomáticamente
+error_11: presentaran → presentarán
+error_12: negandoles → negándoles</t>
+  </si>
+  <si>
+    <t>error_1: indeminzación → indemnización
+error_2: Soquimich → SQM</t>
+  </si>
+  <si>
+    <t>error_1: oficianas → oficinas
+error_2: publico → público
+error_3: asi → así
+error_4: proteccion → protección
+error_5: peronas → personas
+error_6: activiades → actividades
+error_7: alimentacion → alimentación
+error_8: ansioliticos → ansiolíticos
+error_9: poblacion → población
+error_10: sugerian → sugerían
+error_11: estres → estrés</t>
+  </si>
+  <si>
+    <t>error_1: activdades → actividades
+error_2: escenciales → esenciales
+error_3: disminur → disminuir
+error_4: su → sus
+error_5: continuen → continúen
+error_6: ministerio → Ministerio
+error_7: ocpuar → ocupar
+error_8: si → sí
+error_9: evalución → evaluación
+error_10: comeinzo → comienzo
+error_11: resguardar → resguardar</t>
+  </si>
+  <si>
+    <t>error_1: alchol → alcohol
+error_2: rrallado → rallado
+error_3: obeja → oveja
+error_4: girafa → jirafa</t>
+  </si>
+  <si>
+    <t>error_1: prófunda → profunda
+error_2: virsus → virus
+error_3: individuo → individuos
+error_4: antes → ante
+error_5: especificamente → específicamente
+error_6: dónde → donde</t>
+  </si>
+  <si>
+    <t>error_1: covid → COVID
+error_2: mayoria → mayoría
+error_3: paises → países</t>
+  </si>
+  <si>
+    <t>error_1: covid-19 → COVID-19
+error_2: paises → países
+error_3: asotado → azotado
+error_4: ocacionando → ocasionando
+error_5: generalemente → generalmente
+error_6: aún que → aunque
+error_7: santiario → sanitario
+error_8: dificil → difícil</t>
   </si>
   <si>
     <t>error_1: asi → así
@@ -142,93 +229,6 @@
 error_8: que → qué
 error_9: dificil → difícil
 error_10: aún → Aunque</t>
-  </si>
-  <si>
-    <t>error_1: impusado → impulsado</t>
-  </si>
-  <si>
-    <t>error_1: sobretodo → sobre todo
-error_2: solidaridad  → solidaridad
-error_3: tiránica  → tiránica
-error_4: forma de vida de la personas → forma de vida de las personas</t>
-  </si>
-  <si>
-    <t>error_1: relevacia → relevancia
-error_2: debiese → debiese
-error_3: entre ello → entre ellos</t>
-  </si>
-  <si>
-    <t>error_1: llego → llegó
-error_2: frente → enfrenta
-error_3: ultimo → último
-error_4: llamo → llamó
-error_5: super → súper
-error_6: sufienciente → suficiente
-error_7: aun → aún
-error_8: tambien → también
-error_9: prodran → podrán
-error_10: asintomaticamente → asintomáticamente
-error_11: presentaran → presentarán
-error_12: negandoles → negándoles</t>
-  </si>
-  <si>
-    <t>error_1: indeminzación → indemnización
-error_2: Soquimich → SQM</t>
-  </si>
-  <si>
-    <t>error_1: oficianas → oficinas
-error_2: publico → público
-error_3: asi → así
-error_4: proteccion → protección
-error_5: peronas → personas
-error_6: activiades → actividades
-error_7: alimentacion → alimentación
-error_8: ansioliticos → ansiolíticos
-error_9: poblacion → población
-error_10: sugerian → sugerían
-error_11: estres → estrés</t>
-  </si>
-  <si>
-    <t>error_1: activdades → actividades
-error_2: escenciales → esenciales
-error_3: disminur → disminuir
-error_4: su → sus
-error_5: continuen → continúen
-error_6: ministerio → Ministerio
-error_7: ocpuar → ocupar
-error_8: si → sí
-error_9: evalución → evaluación
-error_10: comeinzo → comienzo
-error_11: resguardar → resguardar</t>
-  </si>
-  <si>
-    <t>error_1: alchol → alcohol
-error_2: rrallado → rallado
-error_3: obeja → oveja
-error_4: girafa → jirafa</t>
-  </si>
-  <si>
-    <t>error_1: prófunda → profunda
-error_2: virsus → virus
-error_3: individuo → individuos
-error_4: antes → ante
-error_5: especificamente → específicamente
-error_6: dónde → donde</t>
-  </si>
-  <si>
-    <t>error_1: covid → COVID
-error_2: mayoria → mayoría
-error_3: paises → países</t>
-  </si>
-  <si>
-    <t>error_1: covid-19 → COVID-19
-error_2: paises → países
-error_3: asotado → azotado
-error_4: ocacionando → ocasionando
-error_5: generalemente → generalmente
-error_6: aún que → aunque
-error_7: santiario → sanitario
-error_8: dificil → difícil</t>
   </si>
   <si>
     <t>error_1: presenciales, con → presenciales con

</xml_diff>